<commit_message>
In some placements, the Reinsurance Rate is different (lower) than the Cedent Rate.
</commit_message>
<xml_diff>
--- a/src/main/resources/DebitNoteCalculations.xlsx
+++ b/src/main/resources/DebitNoteCalculations.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jagad\Downloads\Projects\DebitCreditNoteForReinsurance\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FF0ABA-4FF3-4101-B1F0-1889B4FAF5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C642A9BB-5AE8-45BD-9F35-EACD7797AD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ED6B29E6-2EC4-4063-A731-708A46DE0BBC}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Debit Note No.</t>
   </si>
@@ -90,15 +90,6 @@
     <t>Processed</t>
   </si>
   <si>
-    <t>Gross Premium (100%)</t>
-  </si>
-  <si>
-    <t>Share Premium</t>
-  </si>
-  <si>
-    <t>Ceding Comission</t>
-  </si>
-  <si>
     <t>Gross Brokerage Amount</t>
   </si>
   <si>
@@ -111,7 +102,37 @@
     <t>Net Premium Payable To You</t>
   </si>
   <si>
-    <t/>
+    <t>Alibey Maldives Pvt Ltd and/or Joali Maldives Resort</t>
+  </si>
+  <si>
+    <t>18-09-2025 To 17-09-2026</t>
+  </si>
+  <si>
+    <t>RI/25-26/GIFT/D19</t>
+  </si>
+  <si>
+    <t>04th November 2025</t>
+  </si>
+  <si>
+    <t>Ceding Commission (%)</t>
+  </si>
+  <si>
+    <t>Ceding Commission (Amount)</t>
+  </si>
+  <si>
+    <t>Cedent Gross Premium (100%)</t>
+  </si>
+  <si>
+    <t>Cedent Share Premium</t>
+  </si>
+  <si>
+    <t>Reinsurer Gross Premium (100%)</t>
+  </si>
+  <si>
+    <t>Reinsurer Share Premium</t>
+  </si>
+  <si>
+    <t>RI/25-26/GIFT/D20</t>
   </si>
   <si>
     <t>Yes</t>
@@ -121,7 +142,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -502,39 +522,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AED9BEC-AD38-4D6C-B58D-2FBE591B69ED}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.6640625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.21875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.77734375"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="39.5546875"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="23.21875"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="22.5546875"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.0"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.5546875"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="18.88671875"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="9.0"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.77734375"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="21.6640625"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="20.5546875"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="23.6640625"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="34.0"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="23.5546875"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="27.88671875"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="25.88671875"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="35.88671875"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="33.44140625"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="106.44140625"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="89.33203125"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.77734375" customWidth="1"/>
+    <col min="14" max="14" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.6640625" customWidth="1"/>
+    <col min="16" max="16" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="106.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="89.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -569,98 +592,237 @@
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="4"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="1">
         <v>138961467</v>
       </c>
-      <c r="H2" s="0">
+      <c r="H2">
         <v>0.08</v>
       </c>
-      <c r="I2" s="0">
+      <c r="I2">
         <v>0.08</v>
       </c>
-      <c r="J2" s="0">
+      <c r="J2">
         <v>7</v>
       </c>
-      <c r="K2" s="0">
-        <v>27.5</v>
-      </c>
-      <c r="L2" t="n" s="0">
+      <c r="L2">
         <v>111169.17360000001</v>
       </c>
-      <c r="M2" t="n" s="0">
-        <v>7781.842152000001</v>
-      </c>
-      <c r="N2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="O2" t="n" s="0">
-        <v>2140.0065918000005</v>
-      </c>
-      <c r="P2" t="n" s="0">
-        <v>1070.0032959000002</v>
-      </c>
-      <c r="Q2" t="n" s="0">
-        <v>7781.842152000001</v>
-      </c>
-      <c r="R2" t="n" s="0">
-        <v>6711.838856100001</v>
-      </c>
-      <c r="S2" t="s" s="0">
-        <v>26</v>
+      <c r="M2">
+        <v>7781.8421520000011</v>
+      </c>
+      <c r="N2">
+        <v>111169.17360000001</v>
+      </c>
+      <c r="O2">
+        <v>7781.8421520000011</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>7781.8421520000011</v>
+      </c>
+      <c r="U2">
+        <v>7781.8421520000011</v>
+      </c>
+      <c r="V2" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="G3" s="1"/>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="1">
+        <v>183629631.02000001</v>
+      </c>
+      <c r="H3">
+        <v>0.1</v>
+      </c>
+      <c r="I3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J3">
+        <v>13</v>
+      </c>
+      <c r="L3">
+        <v>183629.63102</v>
+      </c>
+      <c r="M3">
+        <v>23871.8520326</v>
+      </c>
+      <c r="N3">
+        <v>128540.74171400003</v>
+      </c>
+      <c r="O3">
+        <v>16710.296422820003</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>23871.8520326</v>
+      </c>
+      <c r="U3">
+        <v>16710.296422820003</v>
+      </c>
+      <c r="V3" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="G4" s="1"/>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="H4">
+        <v>0.2</v>
+      </c>
+      <c r="I4">
+        <v>0.18</v>
+      </c>
+      <c r="J4">
+        <v>15</v>
+      </c>
+      <c r="L4">
+        <v>20000</v>
+      </c>
+      <c r="M4">
+        <v>3000</v>
+      </c>
+      <c r="N4">
+        <v>18000</v>
+      </c>
+      <c r="O4">
+        <v>2700</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>3000</v>
+      </c>
+      <c r="U4">
+        <v>2700</v>
+      </c>
+      <c r="V4" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
multiple Credit notes genration
</commit_message>
<xml_diff>
--- a/src/main/resources/DebitNoteCalculations.xlsx
+++ b/src/main/resources/DebitNoteCalculations.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jagad\Downloads\Projects\DebitCreditNoteForReinsurance\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C642A9BB-5AE8-45BD-9F35-EACD7797AD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08239678-CDA6-4BE2-A741-312D49003EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ED6B29E6-2EC4-4063-A731-708A46DE0BBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CreditNoteDetails" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>Debit Note No.</t>
   </si>
@@ -69,24 +70,12 @@
     <t>Brokerage (%)</t>
   </si>
   <si>
-    <t>RI/25-26/GIFT/D08</t>
-  </si>
-  <si>
-    <t>14th October 2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">Property All Risk </t>
   </si>
   <si>
-    <t>Bunny Holdings (BVI) Ltd – Soneva Fushi Resort</t>
-  </si>
-  <si>
     <t>Solarelle Insurance Pvt. Ltd</t>
   </si>
   <si>
-    <t>30.06.2025 To 30.06.2026</t>
-  </si>
-  <si>
     <t>Processed</t>
   </si>
   <si>
@@ -136,6 +125,30 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Reinsurer Name</t>
+  </si>
+  <si>
+    <t>Reinsurer Share (%)</t>
+  </si>
+  <si>
+    <t>Klapton Re</t>
+  </si>
+  <si>
+    <t>Oman Re</t>
+  </si>
+  <si>
+    <t>Finsbury Re</t>
+  </si>
+  <si>
+    <t>Fac Premium (100%)</t>
+  </si>
+  <si>
+    <t>Share Premium</t>
+  </si>
+  <si>
+    <t>Brokerage (Amount)</t>
   </si>
 </sst>
 </file>
@@ -159,7 +172,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,8 +185,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -196,11 +215,131 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -208,6 +347,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AED9BEC-AD38-4D6C-B58D-2FBE591B69ED}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,37 +743,37 @@
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
@@ -631,46 +782,46 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1">
+        <v>183629631.02000001</v>
+      </c>
+      <c r="H2">
+        <v>0.1</v>
+      </c>
+      <c r="I2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J2">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1">
-        <v>138961467</v>
-      </c>
-      <c r="H2">
-        <v>0.08</v>
-      </c>
-      <c r="I2">
-        <v>0.08</v>
-      </c>
-      <c r="J2">
-        <v>7</v>
-      </c>
       <c r="L2">
-        <v>111169.17360000001</v>
+        <v>183629.63102</v>
       </c>
       <c r="M2">
-        <v>7781.8421520000011</v>
+        <v>23871.8520326</v>
       </c>
       <c r="N2">
-        <v>111169.17360000001</v>
+        <v>128540.74171400003</v>
       </c>
       <c r="O2">
-        <v>7781.8421520000011</v>
+        <v>16710.296422820003</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -685,144 +836,497 @@
         <v>0</v>
       </c>
       <c r="T2">
-        <v>7781.8421520000011</v>
+        <v>23871.8520326</v>
       </c>
       <c r="U2">
-        <v>7781.8421520000011</v>
+        <v>16710.29642282</v>
       </c>
       <c r="V2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="H3">
+        <v>0.2</v>
+      </c>
+      <c r="I3">
+        <v>0.18</v>
+      </c>
+      <c r="J3">
+        <v>15</v>
+      </c>
+      <c r="L3">
+        <v>20000</v>
+      </c>
+      <c r="M3">
+        <v>3000</v>
+      </c>
+      <c r="N3">
+        <v>18000</v>
+      </c>
+      <c r="O3">
+        <v>2700</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>3000</v>
+      </c>
+      <c r="U3">
+        <v>2700</v>
+      </c>
+      <c r="V3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA818891-2FFB-480C-A869-F688B257876A}">
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="H1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="1">
-        <v>183629631.02000001</v>
-      </c>
-      <c r="H3">
-        <v>0.1</v>
-      </c>
-      <c r="I3">
+      <c r="K1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="5">
+        <v>5.5</v>
+      </c>
+      <c r="D2" s="5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="J3">
-        <v>13</v>
-      </c>
-      <c r="L3">
-        <v>183629.63102</v>
-      </c>
-      <c r="M3">
-        <v>23871.8520326</v>
-      </c>
-      <c r="N3">
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="6">
         <v>128540.74171400003</v>
       </c>
-      <c r="O3">
-        <v>16710.296422820003</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>23871.8520326</v>
-      </c>
-      <c r="U3">
-        <v>16710.296422820003</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="I2" s="6">
+        <v>7069.7407942700002</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="12">
+        <v>7069.740794270002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="1">
-        <v>10000000</v>
-      </c>
-      <c r="H4">
-        <v>0.2</v>
-      </c>
-      <c r="I4">
-        <v>0.18</v>
-      </c>
-      <c r="J4">
-        <v>15</v>
-      </c>
-      <c r="L4">
-        <v>20000</v>
-      </c>
-      <c r="M4">
-        <v>3000</v>
-      </c>
-      <c r="N4">
-        <v>18000</v>
-      </c>
-      <c r="O4">
-        <v>2700</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>3000</v>
-      </c>
-      <c r="U4">
-        <v>2700</v>
-      </c>
-      <c r="V4" t="s">
-        <v>33</v>
-      </c>
+      <c r="C3" s="5">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="6">
+        <v>128540.74171400003</v>
+      </c>
+      <c r="I3" s="6">
+        <v>6427.0370857000016</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" s="12">
+        <v>6427.0370857000016</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.08</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="6">
+        <v>146903.70481600001</v>
+      </c>
+      <c r="I4" s="6">
+        <v>3672.5926204000007</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="12">
+        <v>3672.5926204000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="12"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="12"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="12"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="12"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="12"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="12"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="12"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="12"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="12"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="12"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="12"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="12"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="12"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="12"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="12"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="12"/>
+    </row>
+    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added address and reinsured company name in creditNote feature
</commit_message>
<xml_diff>
--- a/src/main/resources/DebitNoteCalculations.xlsx
+++ b/src/main/resources/DebitNoteCalculations.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jagad\Downloads\Projects\DebitCreditNoteForReinsurance\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1375884-62F8-44D7-8197-3C04CCA9186B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D65F78-DA04-4730-ABC5-819C3DDC943D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ED6B29E6-2EC4-4063-A731-708A46DE0BBC}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>Debit Note No.</t>
   </si>
@@ -118,9 +118,6 @@
     <t>Reinsurer Share Premium</t>
   </si>
   <si>
-    <t>RI/25-26/GIFT/D20</t>
-  </si>
-  <si>
     <t>Reinsurer Name</t>
   </si>
   <si>
@@ -158,6 +155,15 @@
   </si>
   <si>
     <t>05-Nov-2025</t>
+  </si>
+  <si>
+    <t>Reinsured Name</t>
+  </si>
+  <si>
+    <t>Reinsurer Address</t>
+  </si>
+  <si>
+    <t>Green City Office Park, Danny Pule Road Lusaka ZM, 10101, Zambia</t>
   </si>
   <si>
     <t>Yes</t>
@@ -167,6 +173,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -390,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -419,6 +426,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,36 +746,36 @@
   <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="L2" sqref="L2:V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.77734375" customWidth="1"/>
-    <col min="14" max="14" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.6640625" customWidth="1"/>
-    <col min="16" max="16" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="106.44140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="89.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.6640625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.33203125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.77734375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="44.0"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.21875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.5546875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.44140625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.5546875"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.88671875"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.0"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.77734375"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="26.77734375"/>
+    <col min="13" max="13" customWidth="true" width="26.77734375"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="28.6640625"/>
+    <col min="15" max="15" customWidth="true" width="28.6640625"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="23.6640625"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="26.5546875"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="34.0"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="23.5546875"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="27.88671875"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="25.88671875"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="35.88671875"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="33.44140625"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="106.44140625"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="89.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -845,7 +855,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
@@ -872,105 +882,63 @@
         <v>13</v>
       </c>
       <c r="K2" s="4"/>
-      <c r="L2" s="5">
+      <c r="L2" s="5" t="n">
         <v>183629.63102</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="5" t="n">
         <v>23871.8520326</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="5" t="n">
         <v>128540.74171400003</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="5" t="n">
         <v>16710.296422820003</v>
       </c>
-      <c r="P2" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>0</v>
-      </c>
-      <c r="R2" s="5">
-        <v>0</v>
-      </c>
-      <c r="S2" s="5">
-        <v>0</v>
-      </c>
-      <c r="T2" s="5">
+      <c r="P2" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q2" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R2" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S2" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T2" s="5" t="n">
         <v>23871.8520326</v>
       </c>
-      <c r="U2" s="5">
+      <c r="U2" s="5" t="n">
         <v>16710.296422820003</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="18">
-        <v>10000000</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="I3" s="4">
-        <v>0.18</v>
-      </c>
-      <c r="J3" s="4">
-        <v>15</v>
-      </c>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="5">
-        <v>20000</v>
-      </c>
-      <c r="M3" s="5">
-        <v>3000</v>
-      </c>
-      <c r="N3" s="5">
-        <v>18000</v>
-      </c>
-      <c r="O3" s="5">
-        <v>2700</v>
-      </c>
-      <c r="P3" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>0</v>
-      </c>
-      <c r="R3" s="5">
-        <v>0</v>
-      </c>
-      <c r="S3" s="5">
-        <v>0</v>
-      </c>
-      <c r="T3" s="5">
-        <v>3000</v>
-      </c>
-      <c r="U3" s="5">
-        <v>2700</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
@@ -1363,446 +1331,488 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA818891-2FFB-480C-A869-F688B257876A}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.6640625"/>
+    <col min="2" max="2" customWidth="true" width="16.6640625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.21875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.44140625"/>
+    <col min="5" max="5" customWidth="true" width="39.33203125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5546875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.88671875"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.77734375"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.88671875"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.44140625"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="18.33203125"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="14.0"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="26.5546875"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="25.88671875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="K1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="M1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="4">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="4">
         <v>5.5</v>
       </c>
-      <c r="E2" s="4">
+      <c r="G2" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F2" s="4">
+      <c r="H2" s="4">
         <v>0</v>
       </c>
-      <c r="G2" s="4">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="5">
-        <v>128540.74171400003</v>
-      </c>
-      <c r="J2" s="5">
+      <c r="I2" s="4"/>
+      <c r="J2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5" t="n">
         <v>7069.740794270002</v>
       </c>
-      <c r="K2" s="5">
-        <v>0</v>
-      </c>
-      <c r="L2" s="5">
-        <v>0</v>
-      </c>
-      <c r="M2" s="11">
+      <c r="M2" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N2" s="5"/>
+      <c r="O2" s="11" t="n">
         <v>7069.740794270002</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="4">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="4">
         <v>5</v>
       </c>
-      <c r="E3" s="4">
+      <c r="G3" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F3" s="4">
+      <c r="H3" s="4">
         <v>0</v>
       </c>
-      <c r="G3" s="4">
-        <v>0</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="5">
-        <v>128540.74171400003</v>
-      </c>
-      <c r="J3" s="5">
-        <v>6427.0370857000016</v>
-      </c>
-      <c r="K3" s="5">
-        <v>0</v>
-      </c>
-      <c r="L3" s="5">
-        <v>0</v>
-      </c>
-      <c r="M3" s="11">
-        <v>6427.0370857000016</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I3" s="4"/>
+      <c r="J3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5" t="n">
+        <v>6427.037085700002</v>
+      </c>
+      <c r="M3" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N3" s="5"/>
+      <c r="O3" s="11" t="n">
+        <v>6427.037085700002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="4">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="4">
         <v>2.5</v>
       </c>
-      <c r="E4" s="4">
+      <c r="G4" s="4">
         <v>0.08</v>
       </c>
-      <c r="F4" s="4">
+      <c r="H4" s="4">
         <v>0</v>
       </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="5">
-        <v>146903.70481600001</v>
-      </c>
-      <c r="J4" s="5">
+      <c r="I4" s="4"/>
+      <c r="J4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5" t="n">
         <v>3672.5926204000007</v>
       </c>
-      <c r="K4" s="5">
-        <v>0</v>
-      </c>
-      <c r="L4" s="5">
-        <v>0</v>
-      </c>
-      <c r="M4" s="11">
+      <c r="M4" s="5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="11" t="n">
         <v>3672.5926204000007</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="20"/>
-      <c r="C5" s="4"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
-      <c r="M5" s="11"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="11"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="20"/>
-      <c r="C6" s="4"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="11"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="11"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="20"/>
-      <c r="C7" s="4"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
-      <c r="M7" s="11"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="11"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="20"/>
-      <c r="C8" s="4"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="11"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="11"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="20"/>
-      <c r="C9" s="4"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
-      <c r="M9" s="11"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="11"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="20"/>
-      <c r="C10" s="4"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
-      <c r="M10" s="11"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="11"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="20"/>
-      <c r="C11" s="4"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-      <c r="M11" s="11"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="11"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="20"/>
-      <c r="C12" s="4"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
-      <c r="M12" s="11"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="11"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="20"/>
-      <c r="C13" s="4"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
-      <c r="M13" s="11"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="11"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="20"/>
-      <c r="C14" s="4"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="11"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="11"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="20"/>
-      <c r="C15" s="4"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
-      <c r="M15" s="11"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="11"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="20"/>
-      <c r="C16" s="4"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
-      <c r="M16" s="11"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="11"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="20"/>
-      <c r="C17" s="4"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
-      <c r="M17" s="11"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="11"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="20"/>
-      <c r="C18" s="4"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
-      <c r="M18" s="11"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="11"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="20"/>
-      <c r="C19" s="4"/>
+      <c r="C19" s="20"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
-      <c r="M19" s="11"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="11"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="20"/>
-      <c r="C20" s="4"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
-      <c r="M20" s="11"/>
-    </row>
-    <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="11"/>
+    </row>
+    <row r="21" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12"/>
       <c r="B21" s="21"/>
-      <c r="C21" s="13"/>
+      <c r="C21" s="21"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
-      <c r="M21" s="15"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>